<commit_message>
Continued excel generation; subsubgroups
</commit_message>
<xml_diff>
--- a/templates/excel/visitExcelSelfMade.xlsx
+++ b/templates/excel/visitExcelSelfMade.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Manu/IdeaProjects/MetaDBRestAPIPadim/templates/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF7F192B-05D4-6A48-8C01-535D74254FD3}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7354BA7-CD18-3443-862C-5508E6EF0140}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="460" windowWidth="38400" windowHeight="23540" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="23540" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Group" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
   <si>
     <t>ID</t>
   </si>
@@ -84,6 +84,9 @@
   </si>
   <si>
     <t>Abbildungen</t>
+  </si>
+  <si>
+    <t>peter</t>
   </si>
 </sst>
 </file>
@@ -588,15 +591,15 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:E1"/>
   <sheetViews>
-    <sheetView zoomScale="202" zoomScaleNormal="202" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView tabSelected="1" zoomScale="202" zoomScaleNormal="202" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -608,6 +611,9 @@
       </c>
       <c r="D1" s="3">
         <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -619,7 +625,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:A19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="202" zoomScaleNormal="202" workbookViewId="0">
+    <sheetView zoomScale="202" zoomScaleNormal="202" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="B10" sqref="B10"/>
     </sheetView>

</xml_diff>